<commit_message>
ccdi multifilter script corrected
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_PHS-Accession-phs003111_Gender-Female_Race-Asian.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_PHS-Accession-phs003111_Gender-Female_Race-Asian.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\CCDI scripts\Commons_Automation\InputFiles\CCDI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\CCDI_Ashwini\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BF256B-7C7D-40EE-BEBC-1BB8C1421EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB053C5-AC8E-4736-B956-92E967F3D2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>WebExcel</t>
   </si>
@@ -83,25 +83,6 @@
 coalesce(d.age_at_diagnosis, '') as `Age at diagnosis (days)`,
 coalesce(fo.vital_status, '') as `Vital Status`
 Order by p.participant_id Limit 100</t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;-[:of_participant]-(p:participant)
- WHERE p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']
-        OPTIONAL MATCH (p)&lt;-[:of_diagnosis]-(dg:diagnosis)
-        OPTIONAL MATCH (p)&lt;-[:of_sample]-(sm:sample)
-        OPTIONAL MATCH (p)-[:of_clinical_measure_file_participant]-(cmfp:clinical_measure_file)
-        OPTIONAL MATCH (s)&lt;-[:of_clinical_measure_file]-(cmf:clinical_measure_file)
-        OPTIONAL MATCH (p)&lt;-[:of_radiology_file]-(rf:radiology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_pathology_file]-(pf:pathology_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_methylation_array_file]-(maf:methylation_array_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_single_cell_sequencing_file]-(scsf:single_cell_sequencing_file)
-        OPTIONAL MATCH (sm)&lt;-[:of_sequencing_file]-(sf:sequencing_file)
-        WITH cmfp, cmf, rf, pf, maf, scsf, sf, p, s, sm, dg
-        return
-        count(distinct s.id) as Studies,
-        count(distinct p.id)as Participants,
-        count(distinct sm.id) as Samples,
-        count(distinct cmfp.id) + count(distinct cmf.id) + count(distinct rf.id) + count(distinct pf.id) + count(distinct maf.id) + count(distinct scsf.id) + count(distinct sf.id) as Files</t>
   </si>
   <si>
     <t>MATCH (s:study)&lt;-[:of_participant]-(p:participant)
@@ -123,8 +104,37 @@
         count(distinct cmfp.id) + count(distinct cmf.id) + count(distinct rf.id) + count(distinct pf.id) + count(distinct maf.id) + count(distinct scsf.id) + count(distinct sf.id) as Files</t>
   </si>
   <si>
+    <t xml:space="preserve">MATCH (p:participant)&lt;-[:of_sample]-(sm:sample)
+        MATCH (s:study)&lt;-[:of_participant]-(p)
+WHERE p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']        WITH p, s, sm
+        RETURN DISTINCT
+          sm.sample_id as `Sample ID`,
+          p.participant_id as `Participant ID`,
+          s.study_id as `Study ID`,
+          sm.anatomic_site as `Anatomic Site`,
+          sm.participant_age_at_collection as `Age at Sample Collection`,
+          sm.diagnosis_icd_o as `Sample ICD-O Morphology`,
+          sm.sample_tumor_status as `Sample Tumor Status`,
+          sm.tumor_classification as `Sample Tumor Classification`
+Order by sm.sample_id Limit 100
+          </t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(dia:diagnosis)
+WHERE  p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']
+WITH DISTINCT p, s
+RETURN
+coalesce(p.participant_id, '') AS `Participant ID`,
+coalesce(s.phs_accession, '') AS `Study Accession`,
+coalesce(p.race, '') AS `Race`,
+coalesce(p.gender, '') AS `Gender` ,
+coalesce(p.ethnicity, '') AS `Ethnicity` ,
+coalesce(p.alternate_participant_id, '') AS `Alternate ID`
+Order by p.participant_id Limit 100</t>
+  </si>
+  <si>
     <t>MATCH (st:study)&lt;-[:of_participant]-(p:participant)
-WHERE p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']
+WHERE p.gender IN ['Female'] and p.race in ['Asian'] and st.phs_accession IN ['phs003111']
   with st, count(p) as num_p
         MATCH (st:study)&lt;-[:of_participant]-(participant)&lt;-[:of_diagnosis]-(dg:diagnosis)
         with st, num_p, dg.diagnosis_icd_o as dg_cancers, count(dg.diagnosis_icd_o) as num_cancers
@@ -159,29 +169,14 @@
          CASE WHEN size(file_types) &gt; 5 THEN apoc.text.join(apoc.coll.remove(file_types, 5, 10000), "") + "..."  else apoc.text.join(file_types, "") END as `File Type (Top 5)`,
          apoc.text.join(COLLECT(DISTINCT pub.pubmed_id), ';') as `PubMed ID`,
          apoc.text.join(COLLECT(DISTINCT stp.personnel_name), ';') as `Principal Investigator(s)`,
-         apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (p:participant)&lt;-[:of_sample]-(sm:sample)
-        MATCH (s:study)&lt;-[:of_participant]-(p)
-WHERE p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']        WITH p, s, sm
-        RETURN DISTINCT
-          sm.sample_id as `Sample ID`,
-          p.participant_id as `Participant ID`,
-          s.study_id as `Study ID`,
-          sm.anatomic_site as `Anatomic Site`,
-          sm.participant_age_at_collection as `Age at Sample Collection`,
-          sm.diagnosis_icd_o as `Sample ICD-O Morphology`,
-          sm.sample_tumor_status as `Sample Tumor Status`,
-          sm.tumor_classification as `Sample Tumor Classification`
-Order by sm.sample_id Limit 100
-          </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (file:clinical_measure_file)
+         apoc.text.join(COLLECT(DISTINCT stf.grant_id), ';') as `Grant ID`
+Order by st.study_short_title Limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (file:clinical_measure_file)
 MATCH (p:participant)-[:of_clinical_measure_file_participant]-(file)
 MATCH (st)&lt;-[:of_participant]-(p)
-WHERE p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']
+where st.phs_accession in ['phs003111']
 WITH file, st, p, ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units, toInteger(floor(log(file.file_size)/log(1024))) as i, 2 as precision
 WITH file, st, p,
 file.file_size /(1024^i) AS value, 10^precision AS factor, units[i] as unit
@@ -194,7 +189,7 @@
 CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
 st.study_id AS `Study ID`,
 p.participant_id as `Participant ID`,
-null AS `Sample ID`,
+'' AS `Sample ID`,
 file.dcf_indexd_guid AS `GUID`,
 file.md5sum AS `MD5sum`
 UNION ALL
@@ -218,8 +213,8 @@
 file.file_type AS `File Type`,
 CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
 st.study_id AS `Study ID`,
-null as `Participant ID`,
-null AS `Sample ID`,
+'' as `Participant ID`,
+'' AS `Sample ID`,
 file.dcf_indexd_guid AS `GUID`,
 file.md5sum AS `MD5sum`
 UNION ALL
@@ -299,7 +294,7 @@
 CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS `File Size`,
 st.study_id AS `Study ID`,
 p.participant_id as `Participant ID`,
-null AS `Sample ID`,
+'' AS `Sample ID`,
 file.dcf_indexd_guid AS `GUID`,
 file.md5sum AS `MD5sum`
 UNION ALL
@@ -356,20 +351,7 @@
 sm.sample_id AS `Sample ID`,
 file.dcf_indexd_guid AS `GUID`,
 file.md5sum AS `MD5sum`
- </t>
-  </si>
-  <si>
-    <t>MATCH (s:study)&lt;--(p:participant)&lt;--(dia:diagnosis)
-WHERE  p.gender IN ['Female'] and p.race in ['Asian'] and s.phs_accession IN ['phs003111']
-WITH DISTINCT p, s
-RETURN
-coalesce(p.participant_id, '') AS `Participant ID`,
-coalesce(s.phs_accession, '') AS `Study Accession`,
-coalesce(p.race, '') AS `Race`,
-coalesce(p.gender, '') AS `Gender` ,
-coalesce(p.ethnicity, '') AS `Ethnicity` ,
-coalesce(p.alternate_participant_id, '') AS `Alternate ID`
-Order by p.participant_id Limit 100</t>
+Order by file.file_name Limit 100</t>
   </si>
 </sst>
 </file>
@@ -741,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,10 +758,10 @@
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -796,7 +778,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -810,7 +792,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>13</v>
@@ -827,7 +809,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>

</xml_diff>